<commit_message>
Make changes on plot labels
</commit_message>
<xml_diff>
--- a/data/AWB_Cilia_Morphology_Analysis.xlsx
+++ b/data/AWB_Cilia_Morphology_Analysis.xlsx
@@ -1,17 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phago\Desktop\single_cell_paper\single_cell_github\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC8E43F-600E-4A69-9DE0-0B513FC75136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="AWB_Cilia" sheetId="1" r:id="rId4"/>
+    <sheet name="AWB_Cilia" sheetId="1" r:id="rId1"/>
+    <sheet name="Table2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Normal</t>
   </si>
@@ -74,9 +86,6 @@
   </si>
   <si>
     <t>wdr-31(tm10423); elmd-1;rpi-2;ankr-26</t>
-  </si>
-  <si>
-    <t>WDR-31 Rescue for AWB cilia</t>
   </si>
   <si>
     <t>Normal (%)</t>
@@ -100,54 +109,59 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -157,7 +171,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -173,7 +187,13 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -187,6 +207,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -198,116 +219,85 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -497,23 +487,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.86"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -532,7 +527,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -549,14 +544,14 @@
         <v>7</v>
       </c>
       <c r="E3" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -573,35 +568,35 @@
         <v>38</v>
       </c>
       <c r="E4" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="6">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="C5" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="6">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E5" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -618,14 +613,14 @@
         <v>4</v>
       </c>
       <c r="E6" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -642,140 +637,140 @@
         <v>103</v>
       </c>
       <c r="E7" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="C8" s="6">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="D8" s="6">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="E8" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9">
       <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="7">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="C9" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="7">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="E9" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="C10" s="7">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D10" s="7">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E10" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="12">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C11" s="12">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D11" s="12">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="E11" s="12">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="6">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="C12" s="6">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="D12" s="6">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="E12" s="6">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="C13" s="6">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6">
-        <v>66.0</v>
+        <v>66</v>
       </c>
       <c r="E13" s="6">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9">
       <c r="A14" s="14"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -786,7 +781,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9">
       <c r="A15" s="15"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -797,7 +792,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -808,7 +803,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -819,133 +814,43 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>3</v>
-      </c>
+    <row r="18" spans="1:9">
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19">
-      <c r="A19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="6">
-        <f>18+33+13</f>
-        <v>64</v>
-      </c>
-      <c r="C19" s="6">
-        <f>1+1+0</f>
-        <v>2</v>
-      </c>
-      <c r="D19" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0.0</v>
-      </c>
+    <row r="19" spans="1:9">
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20">
-      <c r="A20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="6">
-        <v>36.0</v>
-      </c>
-      <c r="C20" s="6">
-        <v>15.0</v>
-      </c>
-      <c r="D20" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="E20" s="6">
-        <v>0.0</v>
-      </c>
+    <row r="20" spans="1:9">
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21">
-      <c r="A21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="17">
-        <v>125.0</v>
-      </c>
-      <c r="C21" s="17">
-        <v>23.0</v>
-      </c>
-      <c r="D21" s="17">
-        <v>96.0</v>
-      </c>
-      <c r="E21" s="17">
-        <v>128.0</v>
-      </c>
+    <row r="21" spans="1:9">
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22">
-      <c r="A22" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="C22" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="D22" s="6">
-        <v>26.0</v>
-      </c>
-      <c r="E22" s="6">
-        <v>31.0</v>
-      </c>
+    <row r="22" spans="1:9">
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23">
-      <c r="A23" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="17">
-        <v>29.0</v>
-      </c>
-      <c r="C23" s="17">
-        <v>7.0</v>
-      </c>
-      <c r="D23" s="17">
-        <v>15.0</v>
-      </c>
-      <c r="E23" s="17">
-        <v>38.0</v>
-      </c>
+    <row r="23" spans="1:9">
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -956,7 +861,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -967,7 +872,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -978,7 +883,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -989,96 +894,31 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>3</v>
-      </c>
+    <row r="28" spans="1:9">
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
     </row>
-    <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="6">
-        <f>10+12+19</f>
-        <v>41</v>
-      </c>
-      <c r="C29" s="6">
-        <f>1+0+0</f>
-        <v>1</v>
-      </c>
-      <c r="D29" s="6">
-        <f>+0+1</f>
-        <v>1</v>
-      </c>
-      <c r="E29" s="6">
-        <v>0.0</v>
-      </c>
+    <row r="29" spans="1:9">
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30">
-      <c r="A30" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="7">
-        <v>13.0</v>
-      </c>
-      <c r="C30" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="D30" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="E30" s="7">
-        <v>0.0</v>
-      </c>
+    <row r="30" spans="1:9">
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31">
-      <c r="A31" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="7">
-        <f>5+1+6+9+10+7+6</f>
-        <v>44</v>
-      </c>
-      <c r="C31" s="7">
-        <f>3+2+1+5+4+0+0</f>
-        <v>15</v>
-      </c>
-      <c r="D31" s="7">
-        <f>8+17+11+6+6+36+25+13</f>
-        <v>122</v>
-      </c>
-      <c r="E31" s="7">
-        <f> 5+36+38+23+11</f>
-        <v>113</v>
-      </c>
+    <row r="31" spans="1:9">
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:9">
       <c r="A32" s="8"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1089,7 +929,7 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9">
       <c r="A33" s="8"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1100,10 +940,8 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>21</v>
-      </c>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1113,166 +951,386 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35">
-      <c r="A35" s="21"/>
-      <c r="B35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A741C36-8E23-4190-80DA-1479F6638017}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6">
+        <f>18+33+13</f>
+        <v>64</v>
+      </c>
+      <c r="C2" s="6">
+        <f>1+1+0</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="38.25">
+      <c r="A3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="63.75">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="17">
+        <v>125</v>
+      </c>
+      <c r="C4" s="17">
+        <v>23</v>
+      </c>
+      <c r="D4" s="17">
+        <v>96</v>
+      </c>
+      <c r="E4" s="17">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51">
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6">
+        <v>32</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="63.75">
+      <c r="A6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="17">
+        <v>29</v>
+      </c>
+      <c r="C6" s="17">
+        <v>7</v>
+      </c>
+      <c r="D6" s="17">
+        <v>15</v>
+      </c>
+      <c r="E6" s="17">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECFC889-601F-4D34-8973-8CF6FE4BE3F0}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6">
+        <f>10+12+19</f>
+        <v>41</v>
+      </c>
+      <c r="C2" s="6">
+        <f>1+0+0</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <f>0+1</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.25">
+      <c r="A3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.25">
+      <c r="A4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="7">
+        <f>5+1+6+9+10+7+6</f>
+        <v>44</v>
+      </c>
+      <c r="C4" s="7">
+        <f>3+2+1+5+4+0+0</f>
+        <v>15</v>
+      </c>
+      <c r="D4" s="7">
+        <f>8+17+11+6+6+36+25+13</f>
+        <v>122</v>
+      </c>
+      <c r="E4" s="7">
+        <f>5+36+38+23+11</f>
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A733C3B-87D5-4322-A2EF-9FFC6933D6C6}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="14.25">
+      <c r="A2" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="24">
+        <v>67</v>
+      </c>
+      <c r="C2" s="17">
+        <v>4</v>
+      </c>
+      <c r="D2" s="17">
+        <v>26</v>
+      </c>
+      <c r="E2" s="17">
+        <v>4</v>
+      </c>
+      <c r="F2" s="24">
+        <f>(B2/(B2+C2+D2+E2)*100)</f>
+        <v>66.336633663366342</v>
+      </c>
+      <c r="G2" s="25">
+        <f>(C2/(B2+C2+D2+E2)*100)</f>
+        <v>3.9603960396039604</v>
+      </c>
+      <c r="H2" s="25">
+        <f>(D2/(B2+C2+D2+E2)*100)</f>
+        <v>25.742574257425744</v>
+      </c>
+      <c r="I2" s="26">
+        <f>(E2/(B2+C2+D2+E2)*100)</f>
+        <v>3.9603960396039604</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.25">
+      <c r="A3" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="24">
+        <v>22</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1</v>
+      </c>
+      <c r="D3" s="17">
+        <v>36</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0</v>
+      </c>
+      <c r="F3" s="24">
+        <f>(B3/(B3+C3+D3+E3)*100)</f>
+        <v>37.288135593220339</v>
+      </c>
+      <c r="G3" s="25">
+        <f>(C3/(B3+C3+D3+E3)*100)</f>
+        <v>1.6949152542372881</v>
+      </c>
+      <c r="H3" s="25">
+        <f>(D3/(B3+C3+D3+E3)*100)</f>
+        <v>61.016949152542374</v>
+      </c>
+      <c r="I3" s="26">
+        <f>(E3/(B3+C3+D3+E3)*100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25">
+      <c r="A4" s="23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="24">
-        <v>67.0</v>
-      </c>
-      <c r="C36" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="D36" s="17">
-        <v>26.0</v>
-      </c>
-      <c r="E36" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="F36" s="24">
-        <f t="shared" ref="F36:F39" si="1">(B36/(B36+C36+D36+E36)*100)</f>
-        <v>66.33663366</v>
-      </c>
-      <c r="G36" s="25">
-        <f t="shared" ref="G36:G39" si="2">(C36/(B36+C36+D36+E36)*100)</f>
-        <v>3.96039604</v>
-      </c>
-      <c r="H36" s="25">
-        <f t="shared" ref="H36:H39" si="3">(D36/(B36+C36+D36+E36)*100)</f>
-        <v>25.74257426</v>
-      </c>
-      <c r="I36" s="26">
-        <f t="shared" ref="I36:I39" si="4">(E36/(B36+C36+D36+E36)*100)</f>
-        <v>3.96039604</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="24">
-        <v>22.0</v>
-      </c>
-      <c r="C37" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="D37" s="17">
-        <v>36.0</v>
-      </c>
-      <c r="E37" s="17">
-        <v>0.0</v>
-      </c>
-      <c r="F37" s="24">
-        <f t="shared" si="1"/>
-        <v>37.28813559</v>
-      </c>
-      <c r="G37" s="25">
-        <f t="shared" si="2"/>
-        <v>1.694915254</v>
-      </c>
-      <c r="H37" s="25">
-        <f t="shared" si="3"/>
-        <v>61.01694915</v>
-      </c>
-      <c r="I37" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="23" t="s">
+      <c r="B4" s="28">
+        <v>53</v>
+      </c>
+      <c r="C4" s="17">
+        <v>28</v>
+      </c>
+      <c r="D4" s="17">
+        <v>92</v>
+      </c>
+      <c r="E4" s="17">
+        <v>11</v>
+      </c>
+      <c r="F4" s="24">
+        <f>(B4/(B4+C4+D4+E4)*100)</f>
+        <v>28.804347826086957</v>
+      </c>
+      <c r="G4" s="25">
+        <f>(C4/(B4+C4+D4+E4)*100)</f>
+        <v>15.217391304347828</v>
+      </c>
+      <c r="H4" s="25">
+        <f>(D4/(B4+C4+D4+E4)*100)</f>
+        <v>50</v>
+      </c>
+      <c r="I4" s="26">
+        <f>(E4/(B4+C4+D4+E4)*100)</f>
+        <v>5.9782608695652177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25">
+      <c r="A5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="28">
-        <v>53.0</v>
-      </c>
-      <c r="C38" s="17">
-        <v>28.0</v>
-      </c>
-      <c r="D38" s="17">
-        <v>92.0</v>
-      </c>
-      <c r="E38" s="17">
-        <v>11.0</v>
-      </c>
-      <c r="F38" s="24">
-        <f t="shared" si="1"/>
-        <v>28.80434783</v>
-      </c>
-      <c r="G38" s="25">
-        <f t="shared" si="2"/>
-        <v>15.2173913</v>
-      </c>
-      <c r="H38" s="25">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="I38" s="26">
-        <f t="shared" si="4"/>
-        <v>5.97826087</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="6">
-        <v>64.0</v>
-      </c>
-      <c r="C39" s="17">
-        <v>5.0</v>
-      </c>
-      <c r="D39" s="17">
-        <v>32.0</v>
-      </c>
-      <c r="E39" s="17">
-        <v>2.0</v>
-      </c>
-      <c r="F39" s="24">
-        <f t="shared" si="1"/>
-        <v>62.13592233</v>
-      </c>
-      <c r="G39" s="25">
-        <f t="shared" si="2"/>
-        <v>4.854368932</v>
-      </c>
-      <c r="H39" s="25">
-        <f t="shared" si="3"/>
-        <v>31.06796117</v>
-      </c>
-      <c r="I39" s="26">
-        <f t="shared" si="4"/>
-        <v>1.941747573</v>
+      <c r="B5" s="6">
+        <v>64</v>
+      </c>
+      <c r="C5" s="17">
+        <v>5</v>
+      </c>
+      <c r="D5" s="17">
+        <v>32</v>
+      </c>
+      <c r="E5" s="17">
+        <v>2</v>
+      </c>
+      <c r="F5" s="24">
+        <f>(B5/(B5+C5+D5+E5)*100)</f>
+        <v>62.135922330097081</v>
+      </c>
+      <c r="G5" s="25">
+        <f>(C5/(B5+C5+D5+E5)*100)</f>
+        <v>4.8543689320388346</v>
+      </c>
+      <c r="H5" s="25">
+        <f>(D5/(B5+C5+D5+E5)*100)</f>
+        <v>31.067961165048541</v>
+      </c>
+      <c r="I5" s="26">
+        <f>(E5/(B5+C5+D5+E5)*100)</f>
+        <v>1.9417475728155338</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>